<commit_message>
created an excel sheet with the performances
</commit_message>
<xml_diff>
--- a/results/performances/performances_polar_apolar.xlsx
+++ b/results/performances/performances_polar_apolar.xlsx
@@ -11,6 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="apolar isotropy" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="polar anisotropy" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="polar isotropy" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="all anisotropy" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="all isotropy" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,95 +439,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ei + Alpha + Dipole + Pi</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ei + Alpha + Dipole</t>
+          <t>Ei + Alpha + Pi</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Alpha + Dipole</t>
+          <t>Ei + Alpha</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Alpha + Dipole + Pi</t>
+          <t>Pi + Ei</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pi + Alpha</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.2108254817370543</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3793491622610133</v>
+        <v>0.5265497639688039</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3418258538616912</v>
+        <v>0.9610753334149637</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2154622538444675</v>
+        <v>1.271563834511352</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4582919031113932</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0.3055489869880953</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3320233910124897</v>
+        <v>0.7539364898971267</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5175891612008552</v>
+        <v>0.7465780862731102</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3099075827789245</v>
+        <v>0.9783564291005794</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6453247856342541</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.2534800511804198</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2809519345643381</v>
+        <v>0.8482818073022681</v>
       </c>
       <c r="C4" t="n">
-        <v>0.375393804398327</v>
+        <v>1.082946839015822</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3891850978305191</v>
+        <v>0.9111777761615172</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.5627059711741039</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.2541444994724172</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3690626397914039</v>
+        <v>0.3826688805714364</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3820350294391228</v>
+        <v>1.170002279825135</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2892566927193675</v>
+        <v>1.254272665982813</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4502129087680733</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0.2076097802159532</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2524215509446512</v>
+        <v>0.51639674670516</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3620969116592002</v>
+        <v>0.9637088664367368</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2657215067766542</v>
+        <v>1.049129694500607</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4462339865424551</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,95 +575,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ei + Alpha + Dipole + Pi</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ei + Alpha + Dipole</t>
+          <t>Ei + Alpha + Pi</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Alpha + Dipole</t>
+          <t>Ei + Alpha</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Alpha + Dipole + Pi</t>
+          <t>Pi + Ei</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pi + Alpha</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.3321349716619197</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4477577797951195</v>
+        <v>0.5626601962334903</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4083421828570664</v>
+        <v>0.932495725147756</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4408974775179098</v>
+        <v>1.271563834511352</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4636680943493121</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0.3638766402041535</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4118322651507619</v>
+        <v>0.5271616330798463</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4351820676343802</v>
+        <v>1.011789946258571</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4140239721744264</v>
+        <v>0.9783564291005794</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3870707482702535</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.3210148473180056</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3324928769631271</v>
+        <v>0.9426680533400128</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3671071970855833</v>
+        <v>0.9694174411579096</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3585627950437669</v>
+        <v>0.9111777761615172</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4899423608629933</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.3440934470386112</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3627337999359304</v>
+        <v>0.3190289668897709</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3611304984549407</v>
+        <v>0.8486709838753951</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3683702957459811</v>
+        <v>1.254272665982813</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4234874674772652</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0.2877024134822573</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3325173805703944</v>
+        <v>0.488580156572951</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3590381502466007</v>
+        <v>0.9063687251534668</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3595235085012145</v>
+        <v>1.049129694500607</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3882818462850995</v>
       </c>
     </row>
   </sheetData>
@@ -650,7 +702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,95 +711,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Ei + Alpha + Dipole + Pi</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Ei + Alpha + Dipole</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Alpha + Dipole</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Alpha + Dipole + Pi</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.2152276859145625</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.59951976322566</v>
+        <v>0.2108254817370543</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4020997742751305</v>
+        <v>0.3793491622610133</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1948498644656363</v>
+        <v>0.3418258538616912</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2154622538444675</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0.2637070494491611</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8449949146977472</v>
+        <v>0.3055489869880953</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4947970364806629</v>
+        <v>0.3320233910124897</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3224539525264279</v>
+        <v>0.5175891612008552</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3099075827789245</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0.3707633288011138</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4662531522940735</v>
+        <v>0.2534800511804198</v>
       </c>
       <c r="C4" t="n">
-        <v>0.457587715842526</v>
+        <v>0.2809519345643381</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4289947940047193</v>
+        <v>0.375393804398327</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.3891850978305191</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0.2651304380493411</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5395860301353854</v>
+        <v>0.2541444994724172</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4866719311209929</v>
+        <v>0.3690626397914039</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2775617324526775</v>
+        <v>0.3820350294391228</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2892566927193675</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0.2000430580789068</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5689972952765208</v>
+        <v>0.2076097802159532</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4197662330536388</v>
+        <v>0.2524215509446512</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2520192417944014</v>
+        <v>0.3620969116592002</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2657215067766542</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +838,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,94 +847,391 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Ei + Alpha + Dipole + Pi</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ei + Alpha + Dipole</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Alpha + Dipole</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Alpha + Dipole + Pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.3321349716619197</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.4477577797951195</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4083421828570664</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4408974775179098</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.3638766402041535</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4118322651507619</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4351820676343802</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.4140239721744264</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.3210148473180056</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3324928769631271</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3671071970855833</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.3585627950437669</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3440934470386112</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3627337999359304</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3611304984549407</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3683702957459811</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.2877024134822573</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3325173805703944</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.3590381502466007</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3595235085012145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Ei + Alpha + Dipole + Pi</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Ei + Alpha + Dipole</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Alpha + Dipole</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Alpha + Dipole + Pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.2152276859145625</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.59951976322566</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4020997742751305</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1948498644656363</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.2637070494491611</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8449949146977472</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4947970364806629</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.3224539525264279</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.3707633288011138</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.4662531522940735</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.457587715842526</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4289947940047193</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2651304380493411</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5395860301353854</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.4866719311209929</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2775617324526775</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.2000430580789068</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5689972952765208</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4197662330536388</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2520192417944014</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ei + Alpha + Dipole + Pi</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Ei + Alpha + Dipole</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Alpha + Dipole</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Alpha + Dipole + Pi</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>poly</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>0.3470499220251377</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>0.5040248465377545</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0.3650544642875731</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.3441594007058143</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>svr</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>0.3504179712992437</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>0.5823934342922048</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.4141216693794856</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.3166355566482289</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>xgb</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0.3106855463025898</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>0.4769994961412236</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.4384711290856459</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.428689951218051</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>nn</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0.5304828493332466</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>0.4778160486610435</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.4053688631875019</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.3869492856871732</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>stacked</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>0.3395245737205701</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0.4451432876186266</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0.3609772571659764</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.3256863613147857</v>
       </c>
     </row>

</xml_diff>